<commit_message>
Lexico teminado para testing
</commit_message>
<xml_diff>
--- a/input/Matriz_Lexico.xlsx
+++ b/input/Matriz_Lexico.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseb\Music\Lexico\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0E719A-2DA0-42E5-89CE-CE6A731C9BCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B824750D-7A47-4076-AAF7-07491FDD4D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{74341061-4426-44B9-B443-0282A79B87A7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8794" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8794" uniqueCount="193">
   <si>
     <t>Estado</t>
   </si>
@@ -616,9 +616,6 @@
   <si>
     <t>q88</t>
   </si>
-  <si>
-    <t>q998</t>
-  </si>
 </sst>
 </file>
 
@@ -1012,8 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AF9BE35-1A03-4ED0-BF66-6378B4FF655B}">
   <dimension ref="A1:BJ142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="E117" sqref="E117"/>
+    <sheetView tabSelected="1" topLeftCell="AD67" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="AT91" sqref="AT91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17514,7 +17511,7 @@
         <v>190</v>
       </c>
       <c r="AT88" s="1" t="s">
-        <v>190</v>
+        <v>88</v>
       </c>
       <c r="AU88" s="1" t="s">
         <v>190</v>
@@ -18078,7 +18075,7 @@
         <v>190</v>
       </c>
       <c r="AT91" s="1" t="s">
-        <v>190</v>
+        <v>88</v>
       </c>
       <c r="AU91" s="1" t="s">
         <v>190</v>
@@ -18308,13 +18305,13 @@
         <v>91</v>
       </c>
       <c r="BH92" s="1" t="s">
-        <v>193</v>
+        <v>88</v>
       </c>
       <c r="BI92" s="1" t="s">
-        <v>193</v>
+        <v>88</v>
       </c>
       <c r="BJ92" s="1" t="s">
-        <v>193</v>
+        <v>88</v>
       </c>
     </row>
     <row r="93" spans="1:62" x14ac:dyDescent="0.25">
@@ -27725,11 +27722,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="8cd9e36f-2d2c-4369-bbf0-c91cd6e84276" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -27889,20 +27887,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="8cd9e36f-2d2c-4369-bbf0-c91cd6e84276" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC2046C7-E4CD-4ED2-8C43-83A9ABB32AFC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCB563C3-64B5-4EF2-82BF-01EAB2F8BED2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8cd9e36f-2d2c-4369-bbf0-c91cd6e84276"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -27926,9 +27921,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCB563C3-64B5-4EF2-82BF-01EAB2F8BED2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC2046C7-E4CD-4ED2-8C43-83A9ABB32AFC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8cd9e36f-2d2c-4369-bbf0-c91cd6e84276"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Implemetacion de errores (Primera version)
</commit_message>
<xml_diff>
--- a/input/Matriz_Lexico.xlsx
+++ b/input/Matriz_Lexico.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseb\Music\Lexico\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Escuela\7mo_semestre\Lenguajes y automatas 1\Analizador_Lexico\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B824750D-7A47-4076-AAF7-07491FDD4D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBA79F6-3FC6-4582-B978-44D036B0261C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{74341061-4426-44B9-B443-0282A79B87A7}"/>
+    <workbookView xWindow="-23148" yWindow="2856" windowWidth="23256" windowHeight="12456" xr2:uid="{74341061-4426-44B9-B443-0282A79B87A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8794" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8794" uniqueCount="194">
   <si>
     <t>Estado</t>
   </si>
@@ -616,6 +616,9 @@
   <si>
     <t>q88</t>
   </si>
+  <si>
+    <t>q998</t>
+  </si>
 </sst>
 </file>
 
@@ -1009,11 +1012,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AF9BE35-1A03-4ED0-BF66-6378B4FF655B}">
   <dimension ref="A1:BJ142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD67" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="AT91" sqref="AT91"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="A131" sqref="A131"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="11.42578125" style="1"/>
   </cols>
@@ -17003,85 +17006,85 @@
         <v>67</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>186</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="J86" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="K86" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="L86" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="M86" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="N86" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="O86" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="P86" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="Q86" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="R86" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="S86" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="T86" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="U86" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="V86" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="W86" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="X86" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="Y86" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="Z86" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AA86" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AB86" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AC86" s="1" t="s">
         <v>67</v>
@@ -17191,85 +17194,85 @@
         <v>188</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="K87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="L87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="M87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="N87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="O87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="P87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="Q87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="R87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="S87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="T87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="U87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="V87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="W87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="X87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="Y87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="Z87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AA87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AB87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AC87" s="1" t="s">
         <v>189</v>
@@ -17302,67 +17305,67 @@
         <v>189</v>
       </c>
       <c r="AM87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AN87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AO87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AP87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AQ87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AR87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AS87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AT87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AU87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AV87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AW87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AX87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AY87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AZ87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="BA87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="BB87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="BC87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="BD87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="BE87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="BF87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="BG87" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="BH87" s="1" t="s">
         <v>88</v>
@@ -17379,85 +17382,85 @@
         <v>189</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>186</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="I88" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="K88" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="L88" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="M88" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="N88" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="O88" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="P88" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="Q88" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="R88" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="S88" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="T88" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="U88" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="V88" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="W88" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="X88" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="Y88" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="Z88" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AA88" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AB88" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AC88" s="1" t="s">
         <v>189</v>
@@ -17567,85 +17570,85 @@
         <v>186</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="K89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="L89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="M89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="N89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="O89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="P89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="Q89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="R89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="S89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="T89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="U89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="V89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="W89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="X89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="Y89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="Z89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AA89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AB89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AC89" s="1" t="s">
         <v>191</v>
@@ -17678,34 +17681,34 @@
         <v>191</v>
       </c>
       <c r="AM89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AN89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AO89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AP89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AQ89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AR89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AS89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AT89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AU89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AV89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AW89" s="1" t="s">
         <v>192</v>
@@ -17714,31 +17717,31 @@
         <v>192</v>
       </c>
       <c r="AY89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AZ89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="BA89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="BB89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="BC89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="BD89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="BE89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="BF89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="BG89" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="BH89" s="1" t="s">
         <v>88</v>
@@ -17755,85 +17758,85 @@
         <v>192</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="K90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="L90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="M90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="N90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="O90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="P90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="Q90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="R90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="S90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="T90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="U90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="V90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="W90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="X90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="Y90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="Z90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AA90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AB90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AC90" s="1" t="s">
         <v>191</v>
@@ -17866,67 +17869,67 @@
         <v>191</v>
       </c>
       <c r="AM90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AN90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AO90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AP90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AQ90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AR90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AS90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AT90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AU90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AV90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AW90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AX90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AY90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AZ90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="BA90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="BB90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="BC90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="BD90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="BE90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="BF90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="BG90" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="BH90" s="1" t="s">
         <v>88</v>
@@ -17943,85 +17946,85 @@
         <v>191</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="J91" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="K91" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="L91" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="M91" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="N91" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="O91" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="P91" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="Q91" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="R91" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="S91" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="T91" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="U91" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="V91" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="W91" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="X91" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="Y91" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="Z91" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AA91" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AB91" s="1" t="s">
-        <v>88</v>
+        <v>193</v>
       </c>
       <c r="AC91" s="1" t="s">
         <v>191</v>
@@ -27722,12 +27725,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="8cd9e36f-2d2c-4369-bbf0-c91cd6e84276" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -27887,17 +27889,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="8cd9e36f-2d2c-4369-bbf0-c91cd6e84276" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCB563C3-64B5-4EF2-82BF-01EAB2F8BED2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC2046C7-E4CD-4ED2-8C43-83A9ABB32AFC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8cd9e36f-2d2c-4369-bbf0-c91cd6e84276"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -27921,11 +27926,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC2046C7-E4CD-4ED2-8C43-83A9ABB32AFC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCB563C3-64B5-4EF2-82BF-01EAB2F8BED2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8cd9e36f-2d2c-4369-bbf0-c91cd6e84276"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>